<commit_message>
Registration testcase's modification with validation.
</commit_message>
<xml_diff>
--- a/TestExcelData/TestData.xlsx
+++ b/TestExcelData/TestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="104">
   <si>
     <t>Password</t>
   </si>
@@ -205,12 +205,6 @@
   </si>
   <si>
     <t>#ba.com</t>
-  </si>
-  <si>
-    <t>Submit</t>
-  </si>
-  <si>
-    <t>cancle</t>
   </si>
   <si>
     <t>My Organization</t>
@@ -328,23 +322,35 @@
     <t>Agency</t>
   </si>
   <si>
-    <t>Email id is invalid, Confirm Password is not same as Password, Password length should be Greater than 8, Website is invalid,</t>
-  </si>
-  <si>
-    <t>Email id is invalid,First Name is invalid,Confirm Password is not same as Password,Contact Number Invalid,Website is invalid,</t>
-  </si>
-  <si>
     <t>Email id is invalid, Special Charater Not allowed, Confirm Password is not same as Password, Contact Number length should be less than 16, Website is invalid, Pincode Number can't be greater than 16,</t>
   </si>
   <si>
-    <t>Client Type can not be blank, Organization Name can't be blank, First Name can't be blank, Last Name can't be blank, Email Id can't be blank,Password can't be blank, Confirm Password can't be blank, Contact Number can't be blank, Website can't be blank, Address can't be blank, Country Name can't be blank, City Name can't be blank,Pincode Number can't be blank,</t>
+    <t>cancel</t>
+  </si>
+  <si>
+    <t>submit</t>
+  </si>
+  <si>
+    <t>Email id is invalid, Confirm Password is not same as Password, Website is invalid,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Password length should be Greater than 8, Confirm Password is not same as Password, Contact Number Invalid, Website is invalid,</t>
+  </si>
+  <si>
+    <t>Client Type can not be blank, Organization Name cant be blank, First Name can't be blank, Last Name cant be blank, Email Id can't be blank,Password cant be blank, Confirm Password can't be blank, Contact Number can't be blank, Website can't be blank, Address can't be blank, Country Name can't be blank, State Name can't be blank, City Name can't be blank, Pincode Number can't be blank,</t>
+  </si>
+  <si>
+    <t>Select Client Type *</t>
+  </si>
+  <si>
+    <t>Select Country *</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,22 +380,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF5F6F7E"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -435,7 +452,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
@@ -462,37 +479,47 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -798,22 +825,22 @@
         <v>6</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -943,10 +970,10 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -958,10 +985,10 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1050,7 +1077,7 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="7" t="s">
@@ -1071,7 +1098,7 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>41</v>
@@ -1092,7 +1119,7 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>41</v>
@@ -1113,7 +1140,7 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>43</v>
@@ -1136,7 +1163,7 @@
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>41</v>
@@ -1159,7 +1186,7 @@
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>41</v>
@@ -1182,7 +1209,7 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>41</v>
@@ -1203,7 +1230,7 @@
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>56</v>
@@ -1226,8 +1253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2320CBAB-D7A0-4988-822B-F25D30DB6020}">
   <dimension ref="A1:W6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="P7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="A1:V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,367 +1274,365 @@
     <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="103.42578125" customWidth="1"/>
+    <col min="22" max="22" width="103.42578125" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="O1" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="P1" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="Q1" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="R1" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="S1" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="T1" s="16" t="s">
+      <c r="T1" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="U1" s="16" t="s">
+      <c r="U1" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="V1" s="16" t="s">
+      <c r="V1" s="19" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17" t="s">
+    <row r="2" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="V2" s="23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="M3" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="N3" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="O3" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="R3" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="T3" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="U3" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="V3" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="W3" s="16"/>
+    </row>
+    <row r="4" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17" t="s">
+      <c r="G4" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="N4" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="O4" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="P4" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q4" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="19" t="s">
+      <c r="R4" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="S4" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="T4" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="U4" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="V4" s="23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="K5" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="N5" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="O5" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="P5" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="R5" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="S5" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="T5" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="U5" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="V5" s="23" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="V2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="K3" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="L3" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="M3" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="N3" s="18" t="s">
+      <c r="K6" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="M6" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="N6" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="O3" s="17" t="s">
+      <c r="O6" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="P6" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="R6" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="S6" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="T6" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="R3" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="S3" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="T3" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="U3" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="V3" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="W3" s="24"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="K4" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="L4" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="M4" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="N4" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="O4" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="P4" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q4" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="R4" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="S4" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="T4" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="U4" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="V4" s="17" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="G5" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="K5" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="L5" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="M5" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="N5" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="O5" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="P5" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q5" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="R5" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="S5" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="T5" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="U5" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="V5" s="17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="L6" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="M6" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="N6" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="O6" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="P6" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q6" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="R6" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="S6" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="T6" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="U6" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="V6" s="17"/>
+      <c r="U6" s="22"/>
+      <c r="V6" s="23"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Remember me and other changes.
</commit_message>
<xml_diff>
--- a/TestExcelData/TestData.xlsx
+++ b/TestExcelData/TestData.xlsx
@@ -4,14 +4,18 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15765" windowHeight="5880" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15765" windowHeight="5880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="forgotPassword" sheetId="2" r:id="rId2"/>
     <sheet name="ChangePassword" sheetId="3" r:id="rId3"/>
     <sheet name="advertiserRegistration" sheetId="4" r:id="rId4"/>
+    <sheet name="afterChangingPassword" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">afterChangingPassword!$A$2:$H$2</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -22,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="108">
   <si>
     <t>Password</t>
   </si>
@@ -66,9 +70,6 @@
     <t>CurrentPassword</t>
   </si>
   <si>
-    <t>Email sent to your registered Email-ID. Please check your Email.</t>
-  </si>
-  <si>
     <t>ClientType</t>
   </si>
   <si>
@@ -279,25 +280,6 @@
     <t>srinivasarao.r@Dtawrkzcom</t>
   </si>
   <si>
-    <t>srinivasar@Dtawrkz.com</t>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Email Id is invalid</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> Email ID not exist...!!!</t>
-  </si>
-  <si>
     <t>expectedResult</t>
   </si>
   <si>
@@ -344,6 +326,30 @@
   </si>
   <si>
     <t>Select Country *</t>
+  </si>
+  <si>
+    <t>Email Id is invalid</t>
+  </si>
+  <si>
+    <t>Email ID not exist...!!!</t>
+  </si>
+  <si>
+    <t>srinivr@Dtawrkz.com</t>
+  </si>
+  <si>
+    <t>8500991792Ss</t>
+  </si>
+  <si>
+    <t>Old password</t>
+  </si>
+  <si>
+    <t>New password</t>
+  </si>
+  <si>
+    <t>Forget Password</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
@@ -452,11 +458,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -520,6 +525,10 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -804,7 +813,7 @@
   <dimension ref="A2:H6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,96 +827,96 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="G2" s="12" t="s">
+      <c r="C2" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>88</v>
+      <c r="H2" s="11" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13" t="s">
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="14" t="s">
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="13" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="13" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="12" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" s="15" t="s">
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="14" t="s">
         <v>3</v>
       </c>
     </row>
@@ -924,10 +933,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D39F5B6E-EB60-43AC-B0C8-0F22598444A3}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,41 +948,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="28"/>
+      <c r="B2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>86</v>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="31" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -985,33 +992,48 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>14</v>
+        <v>102</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{69F64222-8F77-4ED3-AFCF-8D2D1F2297E6}"/>
-    <hyperlink ref="F3:F4" r:id="rId2" display="srinivasarao.r@Dtawrkz.com" xr:uid="{33802220-6173-4369-A441-20C18CC2BCE1}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{3C4F1043-7E7E-4F18-AE4C-B43D9BD820A2}"/>
-    <hyperlink ref="F3" r:id="rId4" xr:uid="{B8444DAA-043A-452C-8493-5FB2E913531B}"/>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{69F64222-8F77-4ED3-AFCF-8D2D1F2297E6}"/>
+    <hyperlink ref="F4:F5" r:id="rId2" display="srinivasarao.r@Dtawrkz.com" xr:uid="{33802220-6173-4369-A441-20C18CC2BCE1}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{3C4F1043-7E7E-4F18-AE4C-B43D9BD820A2}"/>
+    <hyperlink ref="F4" r:id="rId4" xr:uid="{B8444DAA-043A-452C-8493-5FB2E913531B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -1028,220 +1050,220 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="94.140625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="6" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="94.140625" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="C1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7" t="s">
+      <c r="H6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" s="7" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I6" s="10" t="s">
+      <c r="I7" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="7" t="s">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" s="7"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1253,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2320CBAB-D7A0-4988-822B-F25D30DB6020}">
   <dimension ref="A1:W6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="A1:V6"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1274,365 +1296,365 @@
     <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="103.42578125" style="17" customWidth="1"/>
+    <col min="22" max="22" width="103.42578125" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="V1" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="18" t="s">
+      <c r="D2" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q1" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="R1" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="S1" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="T1" s="18" t="s">
+      <c r="E2" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="V2" s="22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="M3" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="N3" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="O3" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="S3" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="T3" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="U3" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="V3" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="W3" s="15"/>
+    </row>
+    <row r="4" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="U1" s="18" t="s">
+      <c r="G4" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="L4" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="N4" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="V1" s="19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="V2" s="23" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="G3" s="24" t="s">
+      <c r="O4" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q4" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="R4" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="S4" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="T4" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="U4" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="V4" s="22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="K3" s="20" t="s">
+      <c r="J5" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="L5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="N5" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="O5" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="P5" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q5" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="R5" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="S5" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="T5" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="U5" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="V5" s="22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="N6" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="O6" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="L3" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="M3" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="N3" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="O3" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20" t="s">
+      <c r="P6" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="R3" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="S3" s="20" t="s">
+      <c r="Q6" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="R6" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="T3" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="U3" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="V3" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="W3" s="16"/>
-    </row>
-    <row r="4" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="K4" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="L4" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="M4" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="N4" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="O4" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="P4" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q4" s="20" t="s">
+      <c r="S6" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="R4" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="S4" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="T4" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="U4" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="V4" s="23" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="K5" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="L5" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="M5" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="N5" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="O5" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="P5" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q5" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="R5" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="S5" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="T5" s="20" t="s">
+      <c r="T6" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="U5" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="V5" s="23" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="H6" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="K6" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="L6" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="M6" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="N6" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="O6" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="P6" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q6" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="R6" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="S6" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="T6" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="U6" s="22"/>
-      <c r="V6" s="23"/>
+      <c r="U6" s="21"/>
+      <c r="V6" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1648,4 +1670,98 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CA0A81-2F38-4328-9E34-E0A82D22B173}">
+  <dimension ref="A2:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{1FE1272C-07DA-44E4-B9C9-BBE0D110F1F4}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{DA10F440-55AA-4C7A-9E87-BCC60076E40D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Created UI package and classes.
</commit_message>
<xml_diff>
--- a/TestExcelData/TestData.xlsx
+++ b/TestExcelData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15765" windowHeight="5880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15765" windowHeight="5880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -356,7 +356,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -371,12 +371,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -472,20 +466,17 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -494,41 +485,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -827,96 +821,96 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="10" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="10" t="s">
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12" t="s">
+      <c r="G3" s="11"/>
+      <c r="H3" s="11" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="13" t="s">
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="12" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="10" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12" t="s">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="10" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G6" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="14" t="s">
+      <c r="G6" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="13" t="s">
         <v>3</v>
       </c>
     </row>
@@ -970,16 +964,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28" t="s">
+    <row r="2" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="27"/>
+      <c r="B2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="31" t="s">
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="30" t="s">
         <v>1</v>
       </c>
     </row>
@@ -994,7 +988,7 @@
       <c r="F3" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="29" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1009,7 +1003,7 @@
       <c r="F4" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="29" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1044,8 +1038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249A7FAE-4B86-495C-8754-C3AB3066EB31}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,14 +1095,14 @@
       <c r="E2" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="F2" s="8"/>
+      <c r="F2" s="7"/>
       <c r="G2" s="6" t="s">
         <v>49</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="31" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1196,7 +1190,7 @@
       <c r="H6" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="8" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1219,7 +1213,7 @@
       <c r="H7" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="8" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1275,7 +1269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2320CBAB-D7A0-4988-822B-F25D30DB6020}">
   <dimension ref="A1:W6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
@@ -1296,365 +1290,365 @@
     <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="103.42578125" style="16" customWidth="1"/>
+    <col min="22" max="22" width="103.42578125" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="O1" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="17" t="s">
+      <c r="P1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="17" t="s">
+      <c r="Q1" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="17" t="s">
+      <c r="R1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="17" t="s">
+      <c r="S1" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="T1" s="17" t="s">
+      <c r="T1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="U1" s="17" t="s">
+      <c r="U1" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="V1" s="18" t="s">
+      <c r="V1" s="17" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19" t="s">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="27" t="s">
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="21" t="s">
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="V2" s="22" t="s">
+      <c r="V2" s="21" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19" t="s">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="K3" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="L3" s="19" t="s">
+      <c r="K3" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="M3" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="N3" s="20" t="s">
+      <c r="N3" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="O3" s="19" t="s">
+      <c r="O3" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19" t="s">
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="R3" s="19" t="s">
+      <c r="R3" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="19" t="s">
+      <c r="S3" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="T3" s="19" t="s">
+      <c r="T3" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="U3" s="21" t="s">
+      <c r="U3" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="V3" s="22" t="s">
+      <c r="V3" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="W3" s="15"/>
+      <c r="W3" s="14"/>
     </row>
     <row r="4" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19" t="s">
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="20" t="s">
+      <c r="J4" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="L4" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="M4" s="19" t="s">
+      <c r="L4" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="N4" s="21" t="s">
+      <c r="N4" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="O4" s="19" t="s">
+      <c r="O4" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="P4" s="21" t="s">
+      <c r="P4" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="Q4" s="19" t="s">
+      <c r="Q4" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="R4" s="19" t="s">
+      <c r="R4" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="S4" s="19" t="s">
+      <c r="S4" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="T4" s="19" t="s">
+      <c r="T4" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="U4" s="21" t="s">
+      <c r="U4" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="V4" s="22" t="s">
+      <c r="V4" s="21" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19" t="s">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="J5" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="K5" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="L5" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="M5" s="19" t="s">
+      <c r="L5" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="N5" s="24" t="s">
+      <c r="N5" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="O5" s="19" t="s">
+      <c r="O5" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="P5" s="21" t="s">
+      <c r="P5" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="19" t="s">
+      <c r="Q5" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="R5" s="19" t="s">
+      <c r="R5" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="S5" s="19" t="s">
+      <c r="S5" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="T5" s="19" t="s">
+      <c r="T5" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="U5" s="21" t="s">
+      <c r="U5" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="V5" s="22" t="s">
+      <c r="V5" s="21" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19" t="s">
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="J6" s="25" t="s">
+      <c r="J6" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="K6" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="M6" s="19" t="s">
+      <c r="K6" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="N6" s="24" t="s">
+      <c r="N6" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="O6" s="19" t="s">
+      <c r="O6" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="P6" s="21" t="s">
+      <c r="P6" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="Q6" s="19" t="s">
+      <c r="Q6" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="R6" s="19" t="s">
+      <c r="R6" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="S6" s="19" t="s">
+      <c r="S6" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="T6" s="19" t="s">
+      <c r="T6" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="U6" s="21"/>
-      <c r="V6" s="22"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="21"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1726,7 +1720,7 @@
       <c r="E3" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>48</v>
       </c>
       <c r="G3" s="6" t="s">
@@ -1746,7 +1740,7 @@
       <c r="E4" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>48</v>
       </c>
       <c r="G4" s="6" t="s">

</xml_diff>

<commit_message>
Change password edit and some changes.
</commit_message>
<xml_diff>
--- a/TestExcelData/TestData.xlsx
+++ b/TestExcelData/TestData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15765" windowHeight="5880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="108">
   <si>
     <t>Password</t>
   </si>
@@ -157,9 +157,6 @@
     <t>Datawrkz1234</t>
   </si>
   <si>
-    <t>current_password - is invalid</t>
-  </si>
-  <si>
     <t>Expected Message</t>
   </si>
   <si>
@@ -181,21 +178,9 @@
     <t>Datawrkz24</t>
   </si>
   <si>
-    <t>Confirm Password can't be blank</t>
-  </si>
-  <si>
-    <t>Password Must contain Alleast OneUppercase latter, One LowerCase Latter and One one digi</t>
-  </si>
-  <si>
-    <t>Confirm Password is not same as Password</t>
-  </si>
-  <si>
     <t>srinivasarao@datawrkz.com</t>
   </si>
   <si>
-    <t>DatawrkZ1</t>
-  </si>
-  <si>
     <t>P/N</t>
   </si>
   <si>
@@ -350,6 +335,21 @@
   </si>
   <si>
     <t>.</t>
+  </si>
+  <si>
+    <t>Confirm Password is not same as Password;</t>
+  </si>
+  <si>
+    <t>current_password - is invalid;</t>
+  </si>
+  <si>
+    <t>Confirm Password can't be blank;</t>
+  </si>
+  <si>
+    <t>Password can't be blank;</t>
+  </si>
+  <si>
+    <t>Password Must contain Alleast One Uppercase latter, One LowerCase Latter and One one digit;</t>
   </si>
 </sst>
 </file>
@@ -828,22 +828,22 @@
         <v>6</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -855,7 +855,7 @@
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
       <c r="F3" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11" t="s">
@@ -887,7 +887,7 @@
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
       <c r="F5" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>42</v>
@@ -905,7 +905,7 @@
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>40</v>
@@ -949,7 +949,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>35</v>
@@ -986,10 +986,10 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1001,10 +1001,10 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G4" s="29" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1016,10 +1016,10 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1036,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249A7FAE-4B86-495C-8754-C3AB3066EB31}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,7 +1064,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>35</v>
@@ -1082,7 +1082,7 @@
         <v>12</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1093,17 +1093,19 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="7"/>
+        <v>77</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="G2" s="6" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="I2" s="31" t="s">
-        <v>2</v>
+        <v>40</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1114,17 +1116,17 @@
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="6"/>
+        <v>77</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="H3" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>2</v>
+        <v>48</v>
+      </c>
+      <c r="I3" s="31" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1135,17 +1137,17 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="I4" s="6" t="s">
-        <v>51</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1156,19 +1158,17 @@
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="H5" s="6"/>
       <c r="I5" s="6" t="s">
-        <v>43</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1179,19 +1179,19 @@
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>40</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>52</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1202,7 +1202,7 @@
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>40</v>
@@ -1211,53 +1211,32 @@
         <v>40</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>53</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>40</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="I8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1355,10 +1334,10 @@
         <v>26</v>
       </c>
       <c r="U1" s="16" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="V1" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="60" x14ac:dyDescent="0.25">
@@ -1371,10 +1350,10 @@
         <v>37</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
@@ -1387,16 +1366,16 @@
       <c r="O2" s="18"/>
       <c r="P2" s="18"/>
       <c r="Q2" s="26" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="R2" s="18"/>
       <c r="S2" s="18"/>
       <c r="T2" s="18"/>
       <c r="U2" s="20" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="V2" s="21" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -1412,10 +1391,10 @@
         <v>38</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H3" s="18" t="s">
         <v>31</v>
@@ -1424,22 +1403,22 @@
         <v>32</v>
       </c>
       <c r="J3" s="19" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K3" s="18" t="s">
         <v>40</v>
       </c>
       <c r="L3" s="18" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="N3" s="19" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="O3" s="18" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="P3" s="18"/>
       <c r="Q3" s="18" t="s">
@@ -1452,13 +1431,13 @@
         <v>29</v>
       </c>
       <c r="T3" s="18" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="U3" s="20" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="V3" s="21" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="W3" s="14"/>
     </row>
@@ -1472,13 +1451,13 @@
         <v>37</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F4" s="18" t="s">
         <v>27</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H4" s="18" t="s">
         <v>31</v>
@@ -1487,19 +1466,19 @@
         <v>32</v>
       </c>
       <c r="J4" s="19" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K4" s="18" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="L4" s="18" t="s">
         <v>40</v>
       </c>
       <c r="M4" s="18" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="N4" s="20" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="O4" s="18" t="s">
         <v>41</v>
@@ -1517,13 +1496,13 @@
         <v>29</v>
       </c>
       <c r="T4" s="18" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="U4" s="20" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="V4" s="21" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -1536,13 +1515,13 @@
         <v>37</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H5" s="18" t="s">
         <v>31</v>
@@ -1551,22 +1530,22 @@
         <v>32</v>
       </c>
       <c r="J5" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="K5" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="L5" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="N5" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="K5" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="L5" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="M5" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="N5" s="23" t="s">
-        <v>71</v>
-      </c>
       <c r="O5" s="18" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="P5" s="20" t="s">
         <v>29</v>
@@ -1581,13 +1560,13 @@
         <v>29</v>
       </c>
       <c r="T5" s="18" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="U5" s="20" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="V5" s="21" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -1600,13 +1579,13 @@
         <v>37</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F6" s="18" t="s">
         <v>27</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H6" s="18" t="s">
         <v>31</v>
@@ -1615,7 +1594,7 @@
         <v>32</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K6" s="18" t="s">
         <v>40</v>
@@ -1624,10 +1603,10 @@
         <v>40</v>
       </c>
       <c r="M6" s="18" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="N6" s="23" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="O6" s="18" t="s">
         <v>41</v>
@@ -1645,7 +1624,7 @@
         <v>29</v>
       </c>
       <c r="T6" s="18" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="U6" s="20"/>
       <c r="V6" s="21"/>
@@ -1692,22 +1671,22 @@
         <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1715,13 +1694,13 @@
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>40</v>
@@ -1735,19 +1714,19 @@
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dataprovider class implementation .
</commit_message>
<xml_diff>
--- a/TestExcelData/TestData.xlsx
+++ b/TestExcelData/TestData.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="forgotPassword" sheetId="2" r:id="rId2"/>
     <sheet name="ChangePassword" sheetId="3" r:id="rId3"/>
-    <sheet name="advertiserRegistration" sheetId="4" r:id="rId4"/>
+    <sheet name="advertiserRegistration" sheetId="6" r:id="rId4"/>
     <sheet name="afterChangingPassword" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">afterChangingPassword!$A$2:$H$2</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="103">
   <si>
     <t>Password</t>
   </si>
@@ -313,9 +313,6 @@
     <t>Password Must contain Alleast One Uppercase latter, One LowerCase Latter and One one digit;</t>
   </si>
   <si>
-    <t>Client Type can not be blank; Organization Name cant be blank; First Name can't be blank; Last Name cant be blank; Email Id can't be blank; Password cant be blank; Confirm Password can't be blank; Contact Number can't be blank; Website can't be blank; Address can't be blank; Country Name can't be blank; State Name can't be blank; City Name can't be blank; Pincode Number can't be blank;</t>
-  </si>
-  <si>
     <t>Email id is invalid; Confirm Password is not same as Password; Website is invalid;</t>
   </si>
   <si>
@@ -335,6 +332,9 @@
   </si>
   <si>
     <t>Email id is invalid; Special Charater Not allowed; Confirm Password is not same as Password; Contact Number length should be less than 16; Website is invalid; Pincode Number can't be greater than 16;</t>
+  </si>
+  <si>
+    <t>Client Type can not be blank; First Name can't be blank; Email Id can't be blank; Confirm Password can't be blank; Contact Number can't be blank; Website can't be blank; Address can't be blank; Country Name can't be blank; State Name can't be blank; City Name can't be blank; Pincode Number can't be blank;</t>
   </si>
 </sst>
 </file>
@@ -456,7 +456,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -474,17 +474,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -507,10 +498,6 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -538,6 +525,9 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -837,97 +827,97 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="18" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24" t="s">
+      <c r="A3" s="19"/>
+      <c r="B3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="22" t="s">
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24" t="s">
+      <c r="G3" s="19"/>
+      <c r="H3" s="19" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24" t="s">
+      <c r="A4" s="19"/>
+      <c r="B4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24" t="s">
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="19" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24" t="s">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
+      <c r="B6" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="24" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="22" t="s">
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="26" t="s">
-        <v>99</v>
+      <c r="H6" s="21" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -958,69 +948,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28" t="s">
+    <row r="2" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="24" t="s">
-        <v>98</v>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="19" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24" t="s">
+      <c r="A3" s="19"/>
+      <c r="B3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="29" t="s">
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" s="20" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="G4" s="25" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1036,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249A7FAE-4B86-495C-8754-C3AB3066EB31}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F9" sqref="A1:I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,7 +1115,7 @@
       <c r="H3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="16" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1237,23 +1227,6 @@
         <v>55</v>
       </c>
       <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I9" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1262,400 +1235,398 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2320CBAB-D7A0-4988-822B-F25D30DB6020}">
-  <dimension ref="A1:W6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CB4FDCE-5534-49AE-9CD8-33199AC6FFF2}">
+  <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.140625" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="103.42578125" style="8" customWidth="1"/>
+    <col min="22" max="22" width="92.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="R1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="S1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="T1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="U1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="V1" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11" t="s">
+    <row r="2" spans="1:22" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="19" t="s">
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="13" t="s">
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="V2" s="14" t="s">
+      <c r="V2" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="T3" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="U3" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="V3" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11" t="s">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D4" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="11" t="s">
+      <c r="E4" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="R4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="T4" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="U4" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="V4" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G3" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="H3" s="11" t="s">
+      <c r="G5" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" s="11" t="s">
+      <c r="J5" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="L3" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="N3" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11" t="s">
+      <c r="M5" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="P5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="R3" s="11" t="s">
+      <c r="R5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="S3" s="11" t="s">
+      <c r="S5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="T3" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="U3" s="13" t="s">
+      <c r="T5" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="U5" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="V3" s="14" t="s">
+      <c r="V5" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="W3" s="7"/>
-    </row>
-    <row r="4" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11" t="s">
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F4" s="11" t="s">
+      <c r="E6" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G6" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I6" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="L4" s="11" t="s">
+      <c r="J6" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="N4" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="O4" s="11" t="s">
+      <c r="L6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="O6" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="P4" s="13" t="s">
+      <c r="P6" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="Q4" s="11" t="s">
+      <c r="Q6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="R4" s="11" t="s">
+      <c r="R6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="S4" s="11" t="s">
+      <c r="S6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="T4" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="U4" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="V4" s="14" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="N5" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="O5" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="P5" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q5" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="R5" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="S5" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="T5" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="U5" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="V5" s="14" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="L6" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="M6" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="N6" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="O6" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="P6" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q6" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="R6" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="S6" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="T6" s="11" t="s">
+      <c r="T6" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="U6" s="13"/>
-      <c r="V6" s="14"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J3" r:id="rId1" display="s.rinivasaraor5945@gmail.com" xr:uid="{0EF23E97-A0B4-4314-961E-A1A0FD8DD3C6}"/>
-    <hyperlink ref="J4:J5" r:id="rId2" display="s.rinivasaraor5945@gmail.com" xr:uid="{A9D888DB-BDC6-45F4-8706-9DABED072CD2}"/>
-    <hyperlink ref="J4" r:id="rId3" xr:uid="{C6D27D36-3F72-46A9-B1F3-F600EE8884A8}"/>
-    <hyperlink ref="J6" r:id="rId4" xr:uid="{B5029683-95C6-47AB-ABFC-9CC7F0E17516}"/>
-    <hyperlink ref="J5" r:id="rId5" xr:uid="{8F3E6B18-C168-471E-9837-8F657649DDEA}"/>
-    <hyperlink ref="N3" r:id="rId6" location=".com" xr:uid="{FB47F147-4884-4A92-953A-FC95740200C8}"/>
-    <hyperlink ref="N5" r:id="rId7" location="com" xr:uid="{E8BEFDC2-AF86-47C1-8027-CC29AC726EAF}"/>
-    <hyperlink ref="N6" r:id="rId8" xr:uid="{AECA3FBB-A249-4FAD-9FA3-BCCB87058252}"/>
+    <hyperlink ref="J3" r:id="rId1" display="s.rinivasaraor5945@gmail.com" xr:uid="{5C42596A-587F-4470-9F06-DEF50B9FA97F}"/>
+    <hyperlink ref="J4:J5" r:id="rId2" display="s.rinivasaraor5945@gmail.com" xr:uid="{A02EF815-AE83-4B98-85C7-4DB0EB83B618}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{9F846BB3-B550-4B01-A9A4-938D5722FA12}"/>
+    <hyperlink ref="J6" r:id="rId4" xr:uid="{38FA9BD0-524F-41A8-A173-A982AE5C1B06}"/>
+    <hyperlink ref="J5" r:id="rId5" xr:uid="{A07DF154-6EDD-4B51-AE3A-C4387D514AB9}"/>
+    <hyperlink ref="N3" r:id="rId6" location=".com" xr:uid="{3E7CA91A-A5F9-46DB-B6C5-64702DEB38E6}"/>
+    <hyperlink ref="N5" r:id="rId7" location="com" xr:uid="{F431D260-98B8-44E7-8B63-F74F1C7E3178}"/>
+    <hyperlink ref="N6" r:id="rId8" xr:uid="{8FF88FD1-3795-4FF9-B820-5D0302F689FC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId9"/>
@@ -1666,8 +1637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CA0A81-2F38-4328-9E34-E0A82D22B173}">
   <dimension ref="A2:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1681,28 +1652,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="22" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1720,10 +1691,10 @@
         <v>43</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>